<commit_message>
find tenlop - class
</commit_message>
<xml_diff>
--- a/server/src/modules/dataExcel/data/teachers.xlsx
+++ b/server/src/modules/dataExcel/data/teachers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tuluong/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/WorkSpace/StudentCare/server/src/modules/dataExcel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8833D1D7-E9B9-A840-97FA-2089F7DE193A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6474AC1C-58B7-0945-AA84-BD15E9CB41F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="460" windowWidth="27640" windowHeight="16140" xr2:uid="{F7FC6003-1A91-5340-8BC6-3655C4A48D10}"/>
   </bookViews>
@@ -1213,7 +1213,7 @@
   <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>